<commit_message>
edit to fix issues, it will now spit out an index error when complete
</commit_message>
<xml_diff>
--- a/audio time spreadsheet.xlsx
+++ b/audio time spreadsheet.xlsx
@@ -1,42 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adama\Documents\Coding stuff\audio-length-generator\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5561D3-7A78-4D56-B662-AE66DF6B1FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -55,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -335,18 +385,260 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="27.81640625" customWidth="1"/>
-  </cols>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>NABS 1.01 - The Revolution</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>NABS 1.02 - Good Night, Sweet Ladies</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>NABS 1.03 - Random Ghosts</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>NABS 1.04 - The Lights of Skaro</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>NABS 2.01 - The Pyramid of Sutekh</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NABS 2.02 - The Vaults of Osiris</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>NABS 2.03 - The Eye of Horus</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>NABS 2.04 - The Tears of Isis</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>NABS 3.01 - The Library in the Body</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>NABS 3.02 - Planet X</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>NABS 3.03 - The Very Dark Thing</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>NABS 3.04 - The Emporium at the End</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>NABS 4.01 - The City and the Clock</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>NABS 4.02 - Asking For a Friend</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>NABS 4.03 - Truant</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>NABS 4.04 - The True Saviour of the Universe</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>NABS 5.01 - Pride of the Lampian</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>NABS 5.02 - Clear History</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>NABS 5.03 - Dead and Breakfast</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>NABS 5.04 - Burrowed Time</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>NABS 6.01 - Have I Told You Lately</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>NABS 6.02 - The Undying Truth</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>NABS 6.03 - Inertia</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>NABS 6.04 - Gallifrey</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edit to remove the prefixs of names
</commit_message>
<xml_diff>
--- a/audio time spreadsheet.xlsx
+++ b/audio time spreadsheet.xlsx
@@ -392,16 +392,19 @@
   </sheetPr>
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="C192" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="27.81640625" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>NABS 1.01 - The Revolution</t>
+          <t>The Revolution</t>
         </is>
       </c>
       <c r="B1" t="n">
@@ -411,7 +414,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NABS 1.02 - Good Night, Sweet Ladies</t>
+          <t>Good Night, Sweet Ladies</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -421,7 +424,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>NABS 1.03 - Random Ghosts</t>
+          <t>Random Ghosts</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -431,7 +434,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>NABS 1.04 - The Lights of Skaro</t>
+          <t>The Lights of Skaro</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -441,7 +444,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>NABS 2.01 - The Pyramid of Sutekh</t>
+          <t>The Pyramid of Sutekh</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -451,7 +454,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NABS 2.02 - The Vaults of Osiris</t>
+          <t>The Vaults of Osiris</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -461,7 +464,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>NABS 2.03 - The Eye of Horus</t>
+          <t>The Eye of Horus</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -471,7 +474,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>NABS 2.04 - The Tears of Isis</t>
+          <t>The Tears of Isis</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -481,7 +484,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NABS 3.01 - The Library in the Body</t>
+          <t>The Library in the Body</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -491,7 +494,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>NABS 3.02 - Planet X</t>
+          <t>Planet X</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -501,7 +504,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>NABS 3.03 - The Very Dark Thing</t>
+          <t>The Very Dark Thing</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -511,7 +514,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>NABS 3.04 - The Emporium at the End</t>
+          <t>The Emporium at the End</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -521,7 +524,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>NABS 4.01 - The City and the Clock</t>
+          <t>The City and the Clock</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -531,7 +534,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>NABS 4.02 - Asking For a Friend</t>
+          <t>Asking For a Friend</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -541,7 +544,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>NABS 4.03 - Truant</t>
+          <t>Truant</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -551,7 +554,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>NABS 4.04 - The True Saviour of the Universe</t>
+          <t>The True Saviour of the Universe</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -561,7 +564,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>NABS 5.01 - Pride of the Lampian</t>
+          <t>Pride of the Lampian</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -571,7 +574,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>NABS 5.02 - Clear History</t>
+          <t>Clear History</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -581,7 +584,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>NABS 5.03 - Dead and Breakfast</t>
+          <t>Dead and Breakfast</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -591,7 +594,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>NABS 5.04 - Burrowed Time</t>
+          <t>Burrowed Time</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -601,7 +604,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>NABS 6.01 - Have I Told You Lately</t>
+          <t>Have I Told You Lately</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -611,7 +614,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>NABS 6.02 - The Undying Truth</t>
+          <t>The Undying Truth</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -621,7 +624,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>NABS 6.03 - Inertia</t>
+          <t>Inertia</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -631,7 +634,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>NABS 6.04 - Gallifrey</t>
+          <t>Gallifrey</t>
         </is>
       </c>
       <c r="B24" t="n">

</xml_diff>

<commit_message>
small edit renaming audio duration to audio data
</commit_message>
<xml_diff>
--- a/audio time spreadsheet.xlsx
+++ b/audio time spreadsheet.xlsx
@@ -1,33 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adama\Documents\Coding stuff\audio-length-generator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666A6B8B-BF98-40B6-9D98-6B9D8C633D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4800" yWindow="0" windowWidth="14400" windowHeight="7810" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="300" yWindow="0" windowWidth="9780" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>Rictus</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,80 +65,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -385,115 +345,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col width="27.81640625" customWidth="1" min="1" max="1"/>
+    <col min="1" max="1" width="48.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>The Two Rivers</t>
-        </is>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F1" t="s">
+        <v>2</v>
       </c>
-      <c r="H1" t="n">
-        <v>73</v>
+      <c r="H1">
+        <v>76</v>
       </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Beauty on the Inside</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>80</v>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Black Friday</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>78</v>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Firewall</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>77</v>
-      </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
+      <c r="O1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edited so all names are consistent
</commit_message>
<xml_diff>
--- a/audio time spreadsheet.xlsx
+++ b/audio time spreadsheet.xlsx
@@ -1,52 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adama\Documents\Coding stuff\audio-length-generator\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666A6B8B-BF98-40B6-9D98-6B9D8C633D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="0" windowWidth="9780" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="300" yWindow="0" windowWidth="9780" windowHeight="10890" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>2025</t>
-  </si>
-  <si>
-    <t>Rictus</t>
-  </si>
-  <si>
-    <t>93</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -65,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -345,34 +385,775 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="48.90625" customWidth="1"/>
+    <col width="48.90625" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Rictus</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="H1" t="n">
         <v>76</v>
       </c>
-      <c r="O1" t="s">
-        <v>0</v>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>78</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>80</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Maelstrom</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>79</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>6DA 1.01 -The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>79</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>6DA 1.02 -Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>78</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6DA 1.03 -Chronomancer</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>78</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>78</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>80</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Maelstrom</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>79</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>6DA 1.01 -The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>79</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>6DA 1.02 -Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>78</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>6DA 1.03 -Chronomancer</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>78</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>6DA 1.01 - The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>78</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>6DA 1.02 - The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>80</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>6DA 1.03 - Maelstrom</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>79</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>6DA 1.01 -The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>79</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>6DA 1.02 -Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>78</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>6DA 1.03 -Chronomancer</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>78</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>78</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>80</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Maelstrom</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>79</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>79</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>78</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Chronomancer</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>78</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>78</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>80</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Maelstrom</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>79</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>79</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>78</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Chronomancer</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>78</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>78</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>80</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Maelstrom</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>79</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>79</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>78</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Chronomancer</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="n">
+        <v>78</v>
+      </c>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added in the a dr converter map
</commit_message>
<xml_diff>
--- a/audio time spreadsheet.xlsx
+++ b/audio time spreadsheet.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E95" sqref="E95"/>
@@ -1339,10 +1339,6 @@
           <t>Chronomancer</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
           <t>3</t>
@@ -1387,6 +1383,3310 @@
         </is>
       </c>
       <c r="O18" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>78</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>80</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Maelstrom</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>79</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>79</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>78</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Chronomancer</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>78</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>78</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>80</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Maelstrom</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>79</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>79</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>78</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Chronomancer</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>78</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>78</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>80</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Maelstrom</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>79</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>79</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>78</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Chronomancer</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>78</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>78</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>80</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Maelstrom</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>79</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>79</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>78</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Chronomancer</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>78</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>78</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>80</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Maelstrom</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>79</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>79</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>78</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Chronomancer</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>78</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>78</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>80</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Maelstrom</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>79</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>79</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H53" t="n">
+        <v>78</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Chronomancer</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>78</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Thirteenth Doctor</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H55" t="n">
+        <v>78</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v>80</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Maelstrom</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H57" t="n">
+        <v>79</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H58" t="n">
+        <v>79</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H59" t="n">
+        <v>78</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Chronomancer</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H60" t="n">
+        <v>78</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H61" t="n">
+        <v>78</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H62" t="n">
+        <v>80</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Maelstrom</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H63" t="n">
+        <v>79</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H64" t="n">
+        <v>79</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H65" t="n">
+        <v>78</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Chronomancer</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H66" t="n">
+        <v>78</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H67" t="n">
+        <v>78</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H68" t="n">
+        <v>80</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Maelstrom</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H69" t="n">
+        <v>79</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H70" t="n">
+        <v>79</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H71" t="n">
+        <v>78</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Chronomancer</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H72" t="n">
+        <v>78</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>13th Dr</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>Graham, Yaz, Ryan</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>Rosa, Martin, Parks, Fred</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>Krasko</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>Malorie Blackman, Chris Chibnall</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>Mark Tonderai</t>
+        </is>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>The Rotting Deep</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H73" t="n">
+        <v>78</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>5th Dr</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>Tegan, Turlough</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>1st Dr, 2nd Dr, 3rd Dr, Susan, the Brigadier, Sarah, the Tremas Master, Jerricho, Rassilon, K9, 4th Dr, Romana II</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>President, Borusa</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>Terrance Dicks</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>Peter Moffatt</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>The Tides of the Moon</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H74" t="n">
+        <v>80</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>5th Dr</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>Tegan, Turlough</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>1st Dr, 2nd Dr, 3rd Dr, Susan, the Brigadier, Sarah, the Tremas Master, Jerricho, Rassilon, K9, 4th Dr, Romana II</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>President, Borusa</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>Terrance Dicks</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>Peter Moffatt</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Maelstrom</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H75" t="n">
+        <v>79</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>5th Dr</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>Tegan, Turlough</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>1st Dr, 2nd Dr, 3rd Dr, Susan, the Brigadier, Sarah, the Tremas Master, Jerricho, Rassilon, K9, 4th Dr, Romana II</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>President, Borusa</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>Terrance Dicks</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>Peter Moffatt</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>The Mindless Ones</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H76" t="n">
+        <v>79</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>5th Dr</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>Tegan, Turlough</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>1st Dr, 2nd Dr, 3rd Dr, Susan, the Brigadier, Sarah, the Tremas Master, Jerricho, Rassilon, K9, 4th Dr, Romana II</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>President, Borusa</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>Terrance Dicks</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>Peter Moffatt</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Reverse Engineering</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H77" t="n">
+        <v>78</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>5th Dr</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>Tegan, Turlough</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>1st Dr, 2nd Dr, 3rd Dr, Susan, the Brigadier, Sarah, the Tremas Master, Jerricho, Rassilon, K9, 4th Dr, Romana II</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>President, Borusa</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>Terrance Dicks</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>Peter Moffatt</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Chronomancer</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="inlineStr"/>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H78" t="n">
+        <v>78</v>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>5th Dr</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>Tegan, Turlough</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>1st Dr, 2nd Dr, 3rd Dr, Susan, the Brigadier, Sarah, the Tremas Master, Jerricho, Rassilon, K9, 4th Dr, Romana II</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>President, Borusa</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>Terrance Dicks</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>Peter Moffatt</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr">
         <is>
           <t>2022</t>
         </is>

</xml_diff>

<commit_message>
added error catching for if the website it scraps dosent have the variables that we needed
</commit_message>
<xml_diff>
--- a/audio time spreadsheet.xlsx
+++ b/audio time spreadsheet.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O430"/>
+  <dimension ref="A1:O453"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E95" sqref="E95"/>
@@ -19631,10 +19631,6 @@
           <t>Chronomancer</t>
         </is>
       </c>
-      <c r="B430" t="inlineStr"/>
-      <c r="C430" t="inlineStr"/>
-      <c r="D430" t="inlineStr"/>
-      <c r="E430" t="inlineStr"/>
       <c r="F430" t="inlineStr">
         <is>
           <t>3</t>
@@ -19681,6 +19677,1190 @@
       <c r="O430" t="inlineStr">
         <is>
           <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>The Temple of Light</t>
+        </is>
+      </c>
+      <c r="F431" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G431" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H431" t="n">
+        <v>60</v>
+      </c>
+      <c r="I431" t="inlineStr">
+        <is>
+          <t>Vicki</t>
+        </is>
+      </c>
+      <c r="M431" t="inlineStr">
+        <is>
+          <t>Jonathan Morris</t>
+        </is>
+      </c>
+      <c r="N431" t="inlineStr">
+        <is>
+          <t>Lisa Bowerman</t>
+        </is>
+      </c>
+      <c r="O431" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>Stardust and Ashes</t>
+        </is>
+      </c>
+      <c r="F432" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G432" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H432" t="n">
+        <v>76</v>
+      </c>
+      <c r="I432" t="inlineStr">
+        <is>
+          <t>Susan</t>
+        </is>
+      </c>
+      <c r="K432" t="inlineStr">
+        <is>
+          <t>1st Dr, Barbara, Ian</t>
+        </is>
+      </c>
+      <c r="M432" t="inlineStr">
+        <is>
+          <t>Ian Potter</t>
+        </is>
+      </c>
+      <c r="N432" t="inlineStr">
+        <is>
+          <t>Lisa Bowerman</t>
+        </is>
+      </c>
+      <c r="O432" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>The White Ship</t>
+        </is>
+      </c>
+      <c r="F433" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G433" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H433" t="n">
+        <v>78</v>
+      </c>
+      <c r="I433" t="inlineStr">
+        <is>
+          <t>1st Dr</t>
+        </is>
+      </c>
+      <c r="J433" t="inlineStr">
+        <is>
+          <t>Steven</t>
+        </is>
+      </c>
+      <c r="M433" t="inlineStr">
+        <is>
+          <t>Paul Morris</t>
+        </is>
+      </c>
+      <c r="N433" t="inlineStr">
+        <is>
+          <t>Lisa Bowerman</t>
+        </is>
+      </c>
+      <c r="O433" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>The Y Factor</t>
+        </is>
+      </c>
+      <c r="F434" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G434" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H434" t="n">
+        <v>71</v>
+      </c>
+      <c r="I434" t="inlineStr">
+        <is>
+          <t>1st Dr</t>
+        </is>
+      </c>
+      <c r="J434" t="inlineStr">
+        <is>
+          <t>Dodo</t>
+        </is>
+      </c>
+      <c r="L434" t="inlineStr">
+        <is>
+          <t>Sanderson, a fungus</t>
+        </is>
+      </c>
+      <c r="M434" t="inlineStr">
+        <is>
+          <t>Christopher Cooper</t>
+        </is>
+      </c>
+      <c r="N434" t="inlineStr">
+        <is>
+          <t>Lisa Bowerman</t>
+        </is>
+      </c>
+      <c r="O434" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>Dark Watchers of California</t>
+        </is>
+      </c>
+      <c r="F435" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G435" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H435" t="n">
+        <v>36</v>
+      </c>
+      <c r="I435" t="inlineStr">
+        <is>
+          <t>12th Dr</t>
+        </is>
+      </c>
+      <c r="J435" t="inlineStr">
+        <is>
+          <t>Bill Potts</t>
+        </is>
+      </c>
+      <c r="L435" t="inlineStr">
+        <is>
+          <t>Finch</t>
+        </is>
+      </c>
+      <c r="M435" t="inlineStr">
+        <is>
+          <t>Riley Silverman</t>
+        </is>
+      </c>
+      <c r="N435" t="inlineStr">
+        <is>
+          <t>Peter Anghelides</t>
+        </is>
+      </c>
+      <c r="O435" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>Dark Watchers of California</t>
+        </is>
+      </c>
+      <c r="F436" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G436" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H436" t="n">
+        <v>36</v>
+      </c>
+      <c r="I436" t="inlineStr">
+        <is>
+          <t>12th Dr</t>
+        </is>
+      </c>
+      <c r="J436" t="inlineStr">
+        <is>
+          <t>Bill Potts</t>
+        </is>
+      </c>
+      <c r="L436" t="inlineStr">
+        <is>
+          <t>Finch</t>
+        </is>
+      </c>
+      <c r="M436" t="inlineStr">
+        <is>
+          <t>Riley Silverman</t>
+        </is>
+      </c>
+      <c r="N436" t="inlineStr">
+        <is>
+          <t>Peter Anghelides</t>
+        </is>
+      </c>
+      <c r="O436" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>Dark Watchers of California</t>
+        </is>
+      </c>
+      <c r="F437" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G437" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H437" t="n">
+        <v>36</v>
+      </c>
+      <c r="I437" t="inlineStr">
+        <is>
+          <t>12th Dr</t>
+        </is>
+      </c>
+      <c r="J437" t="inlineStr">
+        <is>
+          <t>Bill Potts</t>
+        </is>
+      </c>
+      <c r="L437" t="inlineStr">
+        <is>
+          <t>Finch</t>
+        </is>
+      </c>
+      <c r="M437" t="inlineStr">
+        <is>
+          <t>Riley Silverman</t>
+        </is>
+      </c>
+      <c r="N437" t="inlineStr">
+        <is>
+          <t>Peter Anghelides</t>
+        </is>
+      </c>
+      <c r="O437" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>Dark Watchers of California</t>
+        </is>
+      </c>
+      <c r="F438" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G438" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H438" t="n">
+        <v>36</v>
+      </c>
+      <c r="I438" t="inlineStr">
+        <is>
+          <t>12th Dr</t>
+        </is>
+      </c>
+      <c r="J438" t="inlineStr">
+        <is>
+          <t>Bill Potts</t>
+        </is>
+      </c>
+      <c r="L438" t="inlineStr">
+        <is>
+          <t>Finch</t>
+        </is>
+      </c>
+      <c r="M438" t="inlineStr">
+        <is>
+          <t>Riley Silverman</t>
+        </is>
+      </c>
+      <c r="N438" t="inlineStr">
+        <is>
+          <t>Peter Anghelides</t>
+        </is>
+      </c>
+      <c r="O438" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>When I Say Run</t>
+        </is>
+      </c>
+      <c r="F439" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G439" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H439" t="n">
+        <v>41</v>
+      </c>
+      <c r="I439" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J439" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K439" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L439" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M439" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N439" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O439" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>Rise of the Eukaryans</t>
+        </is>
+      </c>
+      <c r="F440" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G440" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H440" t="n">
+        <v>38</v>
+      </c>
+      <c r="I440" t="inlineStr">
+        <is>
+          <t>11th Dr</t>
+        </is>
+      </c>
+      <c r="L440" t="inlineStr">
+        <is>
+          <t>Eukaryans</t>
+        </is>
+      </c>
+      <c r="M440" t="inlineStr">
+        <is>
+          <t>Daniel Hardcastle</t>
+        </is>
+      </c>
+      <c r="N440" t="inlineStr">
+        <is>
+          <t>Peter Anghelides</t>
+        </is>
+      </c>
+      <c r="O440" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>Ahead of Time</t>
+        </is>
+      </c>
+      <c r="F441" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G441" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H441" t="n">
+        <v>45</v>
+      </c>
+      <c r="I441" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J441" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K441" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L441" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M441" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N441" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O441" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>Emerald Isle</t>
+        </is>
+      </c>
+      <c r="F442" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G442" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H442" t="n">
+        <v>49</v>
+      </c>
+      <c r="I442" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J442" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K442" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L442" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M442" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N442" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O442" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>Dark is the Devil that Walks</t>
+        </is>
+      </c>
+      <c r="F443" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G443" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H443" t="n">
+        <v>44</v>
+      </c>
+      <c r="I443" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J443" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K443" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L443" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M443" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N443" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O443" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>Hooklight 1</t>
+        </is>
+      </c>
+      <c r="F444" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G444" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="H444" t="n">
+        <v>216</v>
+      </c>
+      <c r="I444" t="inlineStr">
+        <is>
+          <t>5th Dr</t>
+        </is>
+      </c>
+      <c r="J444" t="inlineStr">
+        <is>
+          <t>Adric, Nyssa, Tegan</t>
+        </is>
+      </c>
+      <c r="K444" t="inlineStr">
+        <is>
+          <t>8th Dr</t>
+        </is>
+      </c>
+      <c r="L444" t="inlineStr">
+        <is>
+          <t>Nura, Nigh Guard</t>
+        </is>
+      </c>
+      <c r="M444" t="inlineStr">
+        <is>
+          <t>Tim Foley</t>
+        </is>
+      </c>
+      <c r="N444" t="inlineStr">
+        <is>
+          <t>Ken Bentley</t>
+        </is>
+      </c>
+      <c r="O444" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>Missy Part 1</t>
+        </is>
+      </c>
+      <c r="F445" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G445" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H445" t="n">
+        <v>78</v>
+      </c>
+      <c r="I445" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J445" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K445" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L445" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M445" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N445" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O445" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>Dark Watchers of California</t>
+        </is>
+      </c>
+      <c r="F446" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G446" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H446" t="n">
+        <v>36</v>
+      </c>
+      <c r="I446" t="inlineStr">
+        <is>
+          <t>12th Dr</t>
+        </is>
+      </c>
+      <c r="J446" t="inlineStr">
+        <is>
+          <t>Bill Potts</t>
+        </is>
+      </c>
+      <c r="L446" t="inlineStr">
+        <is>
+          <t>Finch</t>
+        </is>
+      </c>
+      <c r="M446" t="inlineStr">
+        <is>
+          <t>Riley Silverman</t>
+        </is>
+      </c>
+      <c r="N446" t="inlineStr">
+        <is>
+          <t>Peter Anghelides</t>
+        </is>
+      </c>
+      <c r="O446" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>When I Say Run</t>
+        </is>
+      </c>
+      <c r="F447" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G447" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H447" t="n">
+        <v>41</v>
+      </c>
+      <c r="I447" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J447" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K447" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L447" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M447" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N447" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O447" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>Rise of the Eukaryans</t>
+        </is>
+      </c>
+      <c r="F448" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G448" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H448" t="n">
+        <v>38</v>
+      </c>
+      <c r="I448" t="inlineStr">
+        <is>
+          <t>11th Dr</t>
+        </is>
+      </c>
+      <c r="L448" t="inlineStr">
+        <is>
+          <t>Eukaryans</t>
+        </is>
+      </c>
+      <c r="M448" t="inlineStr">
+        <is>
+          <t>Daniel Hardcastle</t>
+        </is>
+      </c>
+      <c r="N448" t="inlineStr">
+        <is>
+          <t>Peter Anghelides</t>
+        </is>
+      </c>
+      <c r="O448" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>Ahead of Time</t>
+        </is>
+      </c>
+      <c r="F449" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G449" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H449" t="n">
+        <v>45</v>
+      </c>
+      <c r="I449" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J449" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K449" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L449" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M449" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N449" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O449" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>Emerald Isle</t>
+        </is>
+      </c>
+      <c r="F450" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G450" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H450" t="n">
+        <v>49</v>
+      </c>
+      <c r="I450" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J450" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K450" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L450" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M450" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N450" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O450" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>Dark is the Devil that Walks</t>
+        </is>
+      </c>
+      <c r="F451" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G451" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H451" t="n">
+        <v>44</v>
+      </c>
+      <c r="I451" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J451" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K451" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L451" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M451" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N451" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O451" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>Hooklight 1</t>
+        </is>
+      </c>
+      <c r="F452" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G452" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="H452" t="n">
+        <v>216</v>
+      </c>
+      <c r="I452" t="inlineStr">
+        <is>
+          <t>5th Dr</t>
+        </is>
+      </c>
+      <c r="J452" t="inlineStr">
+        <is>
+          <t>Adric, Nyssa, Tegan</t>
+        </is>
+      </c>
+      <c r="K452" t="inlineStr">
+        <is>
+          <t>8th Dr</t>
+        </is>
+      </c>
+      <c r="L452" t="inlineStr">
+        <is>
+          <t>Nura, Nigh Guard</t>
+        </is>
+      </c>
+      <c r="M452" t="inlineStr">
+        <is>
+          <t>Tim Foley</t>
+        </is>
+      </c>
+      <c r="N452" t="inlineStr">
+        <is>
+          <t>Ken Bentley</t>
+        </is>
+      </c>
+      <c r="O452" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>Missy Part 1</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr"/>
+      <c r="C453" t="inlineStr"/>
+      <c r="D453" t="inlineStr"/>
+      <c r="E453" t="inlineStr"/>
+      <c r="F453" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G453" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H453" t="n">
+        <v>78</v>
+      </c>
+      <c r="I453" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J453" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K453" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L453" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M453" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N453" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O453" t="inlineStr">
+        <is>
+          <t>2025</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changed the input line
</commit_message>
<xml_diff>
--- a/audio time spreadsheet.xlsx
+++ b/audio time spreadsheet.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O475"/>
+  <dimension ref="A1:O503"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E95" sqref="E95"/>
@@ -22061,9 +22061,6 @@
           <t>Missy Part 1</t>
         </is>
       </c>
-      <c r="B475" t="inlineStr"/>
-      <c r="C475" t="inlineStr"/>
-      <c r="D475" t="inlineStr"/>
       <c r="E475" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -22113,6 +22110,1442 @@
         </is>
       </c>
       <c r="O475" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>Hooklight 2</t>
+        </is>
+      </c>
+      <c r="F476" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G476" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="H476" t="n">
+        <v>229</v>
+      </c>
+      <c r="I476" t="inlineStr">
+        <is>
+          <t>5th Dr</t>
+        </is>
+      </c>
+      <c r="J476" t="inlineStr">
+        <is>
+          <t>Adric, Nyssa, Tegan</t>
+        </is>
+      </c>
+      <c r="K476" t="inlineStr">
+        <is>
+          <t>8th Dr</t>
+        </is>
+      </c>
+      <c r="L476" t="inlineStr">
+        <is>
+          <t>Nura, Nigh Guard, Halcyon</t>
+        </is>
+      </c>
+      <c r="M476" t="inlineStr">
+        <is>
+          <t>Tim Foley</t>
+        </is>
+      </c>
+      <c r="N476" t="inlineStr">
+        <is>
+          <t>Ken Bentley</t>
+        </is>
+      </c>
+      <c r="O476" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>The Story Demon</t>
+        </is>
+      </c>
+      <c r="E477" t="inlineStr">
+        <is>
+          <t>The Cosmos and Mrs Clarke</t>
+        </is>
+      </c>
+      <c r="F477" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G477" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H477" t="n">
+        <v>82</v>
+      </c>
+      <c r="I477" t="inlineStr">
+        <is>
+          <t>6th Dr</t>
+        </is>
+      </c>
+      <c r="J477" t="inlineStr">
+        <is>
+          <t>Constance</t>
+        </is>
+      </c>
+      <c r="L477" t="inlineStr">
+        <is>
+          <t>Dalek mutant</t>
+        </is>
+      </c>
+      <c r="M477" t="inlineStr">
+        <is>
+          <t>Julian Richards</t>
+        </is>
+      </c>
+      <c r="N477" t="inlineStr">
+        <is>
+          <t>Samuel Clemens</t>
+        </is>
+      </c>
+      <c r="O477" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>The Key to Many Worlds</t>
+        </is>
+      </c>
+      <c r="E478" t="inlineStr">
+        <is>
+          <t>The Cosmos and Mrs Clarke</t>
+        </is>
+      </c>
+      <c r="F478" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G478" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H478" t="n">
+        <v>88</v>
+      </c>
+      <c r="I478" t="inlineStr">
+        <is>
+          <t>6th Dr</t>
+        </is>
+      </c>
+      <c r="J478" t="inlineStr">
+        <is>
+          <t>Constance</t>
+        </is>
+      </c>
+      <c r="K478" t="inlineStr">
+        <is>
+          <t>Iris, Marco</t>
+        </is>
+      </c>
+      <c r="M478" t="inlineStr">
+        <is>
+          <t>Paul Magrs</t>
+        </is>
+      </c>
+      <c r="N478" t="inlineStr">
+        <is>
+          <t>Samuel Clemens</t>
+        </is>
+      </c>
+      <c r="O478" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>Inconstancy</t>
+        </is>
+      </c>
+      <c r="E479" t="inlineStr">
+        <is>
+          <t>The Cosmos and Mrs Clarke</t>
+        </is>
+      </c>
+      <c r="F479" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G479" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H479" t="n">
+        <v>82</v>
+      </c>
+      <c r="I479" t="inlineStr">
+        <is>
+          <t>6th Dr</t>
+        </is>
+      </c>
+      <c r="J479" t="inlineStr">
+        <is>
+          <t>Constance</t>
+        </is>
+      </c>
+      <c r="L479" t="inlineStr">
+        <is>
+          <t>Claudia Purnell</t>
+        </is>
+      </c>
+      <c r="M479" t="inlineStr">
+        <is>
+          <t>Ian Potter</t>
+        </is>
+      </c>
+      <c r="N479" t="inlineStr">
+        <is>
+          <t>Samuel Clemens</t>
+        </is>
+      </c>
+      <c r="O479" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>Missy Part 2</t>
+        </is>
+      </c>
+      <c r="E480" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F480" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G480" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H480" t="n">
+        <v>77</v>
+      </c>
+      <c r="I480" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J480" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K480" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L480" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M480" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N480" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O480" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>A Forest of All Seasons</t>
+        </is>
+      </c>
+      <c r="E481" t="inlineStr">
+        <is>
+          <t>A Feast of Steven</t>
+        </is>
+      </c>
+      <c r="F481" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G481" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H481" t="n">
+        <v>45</v>
+      </c>
+      <c r="I481" t="inlineStr">
+        <is>
+          <t>1st Dr</t>
+        </is>
+      </c>
+      <c r="J481" t="inlineStr">
+        <is>
+          <t>Steven, Vicki</t>
+        </is>
+      </c>
+      <c r="M481" t="inlineStr">
+        <is>
+          <t>Jacqueline Rayner</t>
+        </is>
+      </c>
+      <c r="N481" t="inlineStr">
+        <is>
+          <t>John Ainsworth</t>
+        </is>
+      </c>
+      <c r="O481" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>The Doctor's Gambit</t>
+        </is>
+      </c>
+      <c r="E482" t="inlineStr">
+        <is>
+          <t>A Feast of Steven</t>
+        </is>
+      </c>
+      <c r="F482" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G482" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H482" t="n">
+        <v>44</v>
+      </c>
+      <c r="I482" t="inlineStr">
+        <is>
+          <t>Steven, Dodo</t>
+        </is>
+      </c>
+      <c r="K482" t="inlineStr">
+        <is>
+          <t>1st Dr</t>
+        </is>
+      </c>
+      <c r="M482" t="inlineStr">
+        <is>
+          <t>Jacqueline Rayner</t>
+        </is>
+      </c>
+      <c r="N482" t="inlineStr">
+        <is>
+          <t>John Ainsworth</t>
+        </is>
+      </c>
+      <c r="O482" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>A Feast of Steven - Behind the Scenes</t>
+        </is>
+      </c>
+      <c r="E483" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F483" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G483" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H483" t="n">
+        <v>26</v>
+      </c>
+      <c r="I483" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J483" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K483" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L483" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M483" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N483" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O483" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>The Remains of Kaerula</t>
+        </is>
+      </c>
+      <c r="E484" t="inlineStr">
+        <is>
+          <t>The Ruins of Kaerula</t>
+        </is>
+      </c>
+      <c r="F484" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H484" t="n">
+        <v>77</v>
+      </c>
+      <c r="I484" t="inlineStr">
+        <is>
+          <t>4th Dr</t>
+        </is>
+      </c>
+      <c r="J484" t="inlineStr">
+        <is>
+          <t>Leela, K9</t>
+        </is>
+      </c>
+      <c r="M484" t="inlineStr">
+        <is>
+          <t>Phil Mulryne</t>
+        </is>
+      </c>
+      <c r="N484" t="inlineStr">
+        <is>
+          <t>Helen Goldwyn, Nicholas Briggs, Jamie Anderson</t>
+        </is>
+      </c>
+      <c r="O484" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>The Ruins of Kaerula</t>
+        </is>
+      </c>
+      <c r="E485" t="inlineStr">
+        <is>
+          <t>The Ruins of Kaerula</t>
+        </is>
+      </c>
+      <c r="F485" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H485" t="n">
+        <v>77</v>
+      </c>
+      <c r="I485" t="inlineStr">
+        <is>
+          <t>4th Dr</t>
+        </is>
+      </c>
+      <c r="J485" t="inlineStr">
+        <is>
+          <t>Leela, K9</t>
+        </is>
+      </c>
+      <c r="M485" t="inlineStr">
+        <is>
+          <t>Phil Mulryne</t>
+        </is>
+      </c>
+      <c r="N485" t="inlineStr">
+        <is>
+          <t>Helen Goldwyn, Nicholas Briggs, Jamie Anderson</t>
+        </is>
+      </c>
+      <c r="O485" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>Cry of the Banshee</t>
+        </is>
+      </c>
+      <c r="E486" t="inlineStr">
+        <is>
+          <t>The Ruins of Kaerula</t>
+        </is>
+      </c>
+      <c r="F486" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H486" t="n">
+        <v>75</v>
+      </c>
+      <c r="I486" t="inlineStr">
+        <is>
+          <t>4th Dr</t>
+        </is>
+      </c>
+      <c r="J486" t="inlineStr">
+        <is>
+          <t>Leela, K9</t>
+        </is>
+      </c>
+      <c r="M486" t="inlineStr">
+        <is>
+          <t>Tim Foley</t>
+        </is>
+      </c>
+      <c r="N486" t="inlineStr">
+        <is>
+          <t>Helen Goldwyn, Nicholas Briggs, Jamie Anderson</t>
+        </is>
+      </c>
+      <c r="O486" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>With the Angels Part 1-2</t>
+        </is>
+      </c>
+      <c r="E487" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F487" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G487" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H487" t="n">
+        <v>64</v>
+      </c>
+      <c r="I487" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J487" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K487" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L487" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M487" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N487" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O487" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>Catastrophix</t>
+        </is>
+      </c>
+      <c r="E488" t="inlineStr">
+        <is>
+          <t>Past Forward</t>
+        </is>
+      </c>
+      <c r="F488" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G488" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H488" t="n">
+        <v>67</v>
+      </c>
+      <c r="I488" t="inlineStr">
+        <is>
+          <t>7th Dr</t>
+        </is>
+      </c>
+      <c r="J488" t="inlineStr">
+        <is>
+          <t>Harry, Naomi, Ray</t>
+        </is>
+      </c>
+      <c r="M488" t="inlineStr">
+        <is>
+          <t>Lizzie Hopley</t>
+        </is>
+      </c>
+      <c r="N488" t="inlineStr">
+        <is>
+          <t>Samuel Clemens</t>
+        </is>
+      </c>
+      <c r="O488" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>With the Angels Part 3-4</t>
+        </is>
+      </c>
+      <c r="E489" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F489" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G489" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H489" t="n">
+        <v>67</v>
+      </c>
+      <c r="I489" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J489" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K489" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L489" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M489" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N489" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O489" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>Missy Part 3</t>
+        </is>
+      </c>
+      <c r="E490" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F490" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G490" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H490" t="n">
+        <v>77</v>
+      </c>
+      <c r="I490" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J490" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K490" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L490" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M490" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N490" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O490" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>The Dead Sea</t>
+        </is>
+      </c>
+      <c r="F491" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G491" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H491" t="n">
+        <v>64</v>
+      </c>
+      <c r="I491" t="inlineStr">
+        <is>
+          <t>War Dr</t>
+        </is>
+      </c>
+      <c r="M491" t="inlineStr">
+        <is>
+          <t>Alfie Shaw</t>
+        </is>
+      </c>
+      <c r="N491" t="inlineStr">
+        <is>
+          <t>Ken Bentley</t>
+        </is>
+      </c>
+      <c r="O491" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>Unit 26</t>
+        </is>
+      </c>
+      <c r="F492" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G492" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H492" t="n">
+        <v>69</v>
+      </c>
+      <c r="I492" t="inlineStr">
+        <is>
+          <t>War Dr</t>
+        </is>
+      </c>
+      <c r="M492" t="inlineStr">
+        <is>
+          <t>Alfie Shaw</t>
+        </is>
+      </c>
+      <c r="N492" t="inlineStr">
+        <is>
+          <t>Ken Bentley</t>
+        </is>
+      </c>
+      <c r="O492" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>Yesterday is Tomorrow and Tomorrow is Today</t>
+        </is>
+      </c>
+      <c r="F493" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G493" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H493" t="n">
+        <v>73</v>
+      </c>
+      <c r="I493" t="inlineStr">
+        <is>
+          <t>War Dr</t>
+        </is>
+      </c>
+      <c r="M493" t="inlineStr">
+        <is>
+          <t>Alfie Shaw</t>
+        </is>
+      </c>
+      <c r="N493" t="inlineStr">
+        <is>
+          <t>Ken Bentley</t>
+        </is>
+      </c>
+      <c r="O493" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>Kaiju</t>
+        </is>
+      </c>
+      <c r="E494" t="inlineStr">
+        <is>
+          <t>Fractures</t>
+        </is>
+      </c>
+      <c r="F494" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H494" t="n">
+        <v>74</v>
+      </c>
+      <c r="I494" t="inlineStr">
+        <is>
+          <t>Bambera, Savarin, Rix</t>
+        </is>
+      </c>
+      <c r="K494" t="inlineStr">
+        <is>
+          <t>McManis</t>
+        </is>
+      </c>
+      <c r="M494" t="inlineStr">
+        <is>
+          <t>Robert Valentine</t>
+        </is>
+      </c>
+      <c r="N494" t="inlineStr">
+        <is>
+          <t>Samuel Clemens</t>
+        </is>
+      </c>
+      <c r="O494" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>Debrief</t>
+        </is>
+      </c>
+      <c r="E495" t="inlineStr">
+        <is>
+          <t>Fractures</t>
+        </is>
+      </c>
+      <c r="F495" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H495" t="n">
+        <v>75</v>
+      </c>
+      <c r="I495" t="inlineStr">
+        <is>
+          <t>Zbrigniev</t>
+        </is>
+      </c>
+      <c r="K495" t="inlineStr">
+        <is>
+          <t>Bambera</t>
+        </is>
+      </c>
+      <c r="L495" t="inlineStr">
+        <is>
+          <t>Brigade Leader, Winifred Bambera</t>
+        </is>
+      </c>
+      <c r="M495" t="inlineStr">
+        <is>
+          <t>Alfie Shaw</t>
+        </is>
+      </c>
+      <c r="N495" t="inlineStr">
+        <is>
+          <t>Samuel Clemens</t>
+        </is>
+      </c>
+      <c r="O495" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>Shatterpoint</t>
+        </is>
+      </c>
+      <c r="E496" t="inlineStr">
+        <is>
+          <t>Fractures</t>
+        </is>
+      </c>
+      <c r="F496" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H496" t="n">
+        <v>72</v>
+      </c>
+      <c r="I496" t="inlineStr">
+        <is>
+          <t>Bambera, Savarin, Rix</t>
+        </is>
+      </c>
+      <c r="M496" t="inlineStr">
+        <is>
+          <t>Mark Wright</t>
+        </is>
+      </c>
+      <c r="N496" t="inlineStr">
+        <is>
+          <t>Samuel Clemens</t>
+        </is>
+      </c>
+      <c r="O496" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>The Voord in London</t>
+        </is>
+      </c>
+      <c r="E497" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F497" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G497" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H497" t="n">
+        <v>84</v>
+      </c>
+      <c r="I497" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J497" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K497" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L497" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M497" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N497" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O497" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>The Thal from G.R.A.C.E</t>
+        </is>
+      </c>
+      <c r="E498" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F498" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G498" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H498" t="n">
+        <v>84</v>
+      </c>
+      <c r="I498" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J498" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K498" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L498" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M498" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N498" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O498" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>Allegiance</t>
+        </is>
+      </c>
+      <c r="E499" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F499" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G499" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H499" t="n">
+        <v>86</v>
+      </c>
+      <c r="I499" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="J499" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K499" t="inlineStr">
+        <is>
+          <t>N, /, A</t>
+        </is>
+      </c>
+      <c r="L499" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M499" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N499" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O499" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>Spoil of War</t>
+        </is>
+      </c>
+      <c r="E500" t="inlineStr">
+        <is>
+          <t>Pursuit</t>
+        </is>
+      </c>
+      <c r="F500" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G500" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H500" t="n">
+        <v>76</v>
+      </c>
+      <c r="I500" t="inlineStr">
+        <is>
+          <t>Alex, Cass</t>
+        </is>
+      </c>
+      <c r="K500" t="inlineStr">
+        <is>
+          <t>8th Dr, Hieronyma Friend</t>
+        </is>
+      </c>
+      <c r="L500" t="inlineStr">
+        <is>
+          <t>Sontarans</t>
+        </is>
+      </c>
+      <c r="M500" t="inlineStr">
+        <is>
+          <t>Mark Wright</t>
+        </is>
+      </c>
+      <c r="N500" t="inlineStr">
+        <is>
+          <t>Ken Bentley</t>
+        </is>
+      </c>
+      <c r="O500" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>The Tale of Alex</t>
+        </is>
+      </c>
+      <c r="E501" t="inlineStr">
+        <is>
+          <t>Pursuit</t>
+        </is>
+      </c>
+      <c r="F501" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G501" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H501" t="n">
+        <v>76</v>
+      </c>
+      <c r="I501" t="inlineStr">
+        <is>
+          <t>Eighth Doctor, Alex, Cass, Hieronyma Friend</t>
+        </is>
+      </c>
+      <c r="M501" t="inlineStr">
+        <is>
+          <t>Katharine Armitage</t>
+        </is>
+      </c>
+      <c r="N501" t="inlineStr">
+        <is>
+          <t>Ken Bentley</t>
+        </is>
+      </c>
+      <c r="O501" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>See-Saw</t>
+        </is>
+      </c>
+      <c r="E502" t="inlineStr">
+        <is>
+          <t>Pursuit</t>
+        </is>
+      </c>
+      <c r="F502" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G502" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H502" t="n">
+        <v>67</v>
+      </c>
+      <c r="I502" t="inlineStr">
+        <is>
+          <t>Eighth Doctor, Alex, Cass, Hieronyma Friend</t>
+        </is>
+      </c>
+      <c r="M502" t="inlineStr">
+        <is>
+          <t>James Moran</t>
+        </is>
+      </c>
+      <c r="N502" t="inlineStr">
+        <is>
+          <t>Ken Bentley</t>
+        </is>
+      </c>
+      <c r="O502" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>The First Forest</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr"/>
+      <c r="C503" t="inlineStr"/>
+      <c r="D503" t="inlineStr"/>
+      <c r="E503" t="inlineStr">
+        <is>
+          <t>Pursuit</t>
+        </is>
+      </c>
+      <c r="F503" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G503" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H503" t="n">
+        <v>76</v>
+      </c>
+      <c r="I503" t="inlineStr">
+        <is>
+          <t>Eighth Doctor, Alex, Cass, Hieronyma Friend</t>
+        </is>
+      </c>
+      <c r="J503" t="inlineStr"/>
+      <c r="K503" t="inlineStr"/>
+      <c r="L503" t="inlineStr"/>
+      <c r="M503" t="inlineStr">
+        <is>
+          <t>Tim Foley</t>
+        </is>
+      </c>
+      <c r="N503" t="inlineStr">
+        <is>
+          <t>Ken Bentley</t>
+        </is>
+      </c>
+      <c r="O503" t="inlineStr">
         <is>
           <t>2025</t>
         </is>

</xml_diff>